<commit_message>
Implement Advance task Nunit Project
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2020\Advance Task\Nunit\marsframework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DE7032-D670-4222-A53C-85DFF4D268FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850BE863-B3C2-4AC7-B538-AE7A3E7665B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>Url</t>
   </si>
@@ -329,6 +329,24 @@
   </si>
   <si>
     <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book.</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>Marathi</t>
+  </si>
+  <si>
+    <t>Speaking</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>ISTQB2</t>
+  </si>
+  <si>
+    <t>Chinese</t>
   </si>
 </sst>
 </file>
@@ -797,10 +815,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EBB194-4BA9-4E67-BE84-069437835BED}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,6 +851,20 @@
         <v>80</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -840,10 +872,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822F18DE-1A89-4A3A-BEFA-D87A2D317EAC}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,6 +912,20 @@
       </c>
       <c r="D2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1058,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD5A18B-557E-4C46-AA42-15D5655047D3}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1453,13 +1499,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A26A70-10D4-4E96-BF40-FC7FF0101EF0}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1475,6 +1525,30 @@
       </c>
       <c r="B2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1484,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B9FA7A-A546-424B-90C3-722A10E30329}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1508,6 +1582,22 @@
         <v>73</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>